<commit_message>
SerenityASM: Version 3.0.1 fix bug about .asciiz
</commit_message>
<xml_diff>
--- a/Scancode-VirtualKeyCode.xlsx
+++ b/Scancode-VirtualKeyCode.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tsinghua\Documents\study\ProfessionalCourse\Assemble_Language&amp;Interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scn3/win10/SerenityTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$179</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="398">
   <si>
     <t>KEY</t>
   </si>
@@ -784,59 +787,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x111</t>
-  </si>
-  <si>
-    <t>0x15b</t>
-  </si>
-  <si>
-    <t>0x112</t>
-  </si>
-  <si>
-    <t>0x15c</t>
-  </si>
-  <si>
-    <t>0x15d</t>
-  </si>
-  <si>
-    <t>0x12d</t>
-  </si>
-  <si>
-    <t>0x124</t>
-  </si>
-  <si>
-    <t>0x121</t>
-  </si>
-  <si>
-    <t>0x12e</t>
-  </si>
-  <si>
-    <t>0x123</t>
-  </si>
-  <si>
-    <t>0x122</t>
-  </si>
-  <si>
-    <t>0x126</t>
-  </si>
-  <si>
-    <t>0x125</t>
-  </si>
-  <si>
-    <t>0x128</t>
-  </si>
-  <si>
-    <t>0x127</t>
-  </si>
-  <si>
-    <t>0x100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1286,6 +1236,10 @@
   </si>
   <si>
     <t>0x00010021</t>
+  </si>
+  <si>
+    <t>0x00010012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1620,20 +1574,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="F146" sqref="F146"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141:D157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="26.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
@@ -1658,10 +1612,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
@@ -1675,10 +1629,10 @@
         <v>215</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
@@ -1686,10 +1640,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -1703,10 +1657,10 @@
         <v>188</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -1720,10 +1674,10 @@
         <v>174</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -1737,10 +1691,10 @@
         <v>159</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -1754,10 +1708,10 @@
         <v>166</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -1771,10 +1725,10 @@
         <v>233</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -1782,10 +1736,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1803,10 +1757,10 @@
         <v>221</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1824,10 +1778,10 @@
         <v>208</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1845,10 +1799,10 @@
         <v>196</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1866,10 +1820,10 @@
         <v>182</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1887,10 +1841,10 @@
         <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1908,21 +1862,21 @@
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
@@ -1930,10 +1884,10 @@
         <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
@@ -1947,10 +1901,10 @@
         <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
@@ -1964,10 +1918,10 @@
         <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
@@ -1975,10 +1929,10 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1996,10 +1950,10 @@
         <v>81</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
@@ -2013,10 +1967,10 @@
         <v>125</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
@@ -2030,10 +1984,10 @@
         <v>205</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
@@ -2041,10 +1995,10 @@
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2056,10 +2010,10 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2071,10 +2025,10 @@
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2092,10 +2046,10 @@
         <v>193</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2113,10 +2067,10 @@
         <v>142</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2134,10 +2088,10 @@
         <v>5</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2155,10 +2109,10 @@
         <v>172</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2176,10 +2130,10 @@
         <v>213</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2188,13 +2142,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2206,10 +2160,10 @@
         <v>20</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2227,10 +2181,10 @@
         <v>18</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
@@ -2244,10 +2198,10 @@
         <v>179</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
@@ -2261,10 +2215,10 @@
         <v>26</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
@@ -2278,10 +2232,10 @@
         <v>33</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>366</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
@@ -2295,10 +2249,10 @@
         <v>225</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>367</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.15">
@@ -2312,10 +2266,10 @@
         <v>219</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.15">
@@ -2323,10 +2277,10 @@
         <v>27</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
@@ -2334,10 +2288,10 @@
         <v>28</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
@@ -2351,10 +2305,10 @@
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
@@ -2368,10 +2322,10 @@
         <v>164</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>369</v>
+        <v>352</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2389,10 +2343,10 @@
         <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>370</v>
+        <v>353</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2410,10 +2364,10 @@
         <v>150</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2431,10 +2385,10 @@
         <v>134</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -2452,10 +2406,10 @@
         <v>231</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2464,13 +2418,13 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -2482,10 +2436,10 @@
         <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2503,10 +2457,10 @@
         <v>102</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.15">
@@ -2520,10 +2474,10 @@
         <v>10</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.15">
@@ -2537,10 +2491,10 @@
         <v>56</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.15">
@@ -2554,10 +2508,10 @@
         <v>49</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.15">
@@ -2571,10 +2525,10 @@
         <v>186</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.15">
@@ -2588,10 +2542,10 @@
         <v>236</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.15">
@@ -2599,10 +2553,10 @@
         <v>37</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -2614,10 +2568,10 @@
         <v>38</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -2629,10 +2583,10 @@
         <v>39</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -2650,10 +2604,10 @@
         <v>95</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -2671,10 +2625,10 @@
         <v>72</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.15">
@@ -2688,10 +2642,10 @@
         <v>157</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.15">
@@ -2705,10 +2659,10 @@
         <v>240</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.15">
@@ -2722,21 +2676,21 @@
         <v>248</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.15">
@@ -2744,10 +2698,10 @@
         <v>40</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.15">
@@ -2761,10 +2715,10 @@
         <v>235</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.15">
@@ -2778,10 +2732,10 @@
         <v>79</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.15">
@@ -2795,10 +2749,10 @@
         <v>64</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.15">
@@ -2812,10 +2766,10 @@
         <v>109</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.15">
@@ -2829,10 +2783,10 @@
         <v>200</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.15">
@@ -2846,10 +2800,10 @@
         <v>6</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.15">
@@ -2857,10 +2811,10 @@
         <v>47</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.15">
@@ -2868,10 +2822,10 @@
         <v>48</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.15">
@@ -2885,10 +2839,10 @@
         <v>238</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.15">
@@ -2902,10 +2856,10 @@
         <v>246</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
@@ -2923,10 +2877,10 @@
         <v>87</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
@@ -2944,10 +2898,10 @@
         <v>224</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
@@ -2965,10 +2919,10 @@
         <v>118</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.15">
@@ -2982,21 +2936,21 @@
         <v>21</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B81" s="1" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.15">
@@ -3004,10 +2958,10 @@
         <v>50</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.15">
@@ -3015,10 +2969,10 @@
         <v>51</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.15">
@@ -3032,10 +2986,10 @@
         <v>229</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.15">
@@ -3043,10 +2997,10 @@
         <v>53</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.15">
@@ -3060,10 +3014,10 @@
         <v>8</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.15">
@@ -3077,10 +3031,10 @@
         <v>28</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.15">
@@ -3088,10 +3042,10 @@
         <v>56</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.15">
@@ -3099,10 +3053,10 @@
         <v>57</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.15">
@@ -3116,10 +3070,10 @@
         <v>66</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.15">
@@ -3133,10 +3087,10 @@
         <v>104</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.15">
@@ -3150,10 +3104,10 @@
         <v>145</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -3171,10 +3125,10 @@
         <v>218</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
@@ -3183,13 +3137,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B94" s="1" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
@@ -3207,10 +3161,10 @@
         <v>36</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
@@ -3219,13 +3173,13 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B96" s="1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
@@ -3234,13 +3188,13 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B97" s="1" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
@@ -3252,10 +3206,10 @@
         <v>60</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
@@ -3267,10 +3221,10 @@
         <v>61</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.15">
@@ -3278,10 +3232,10 @@
         <v>62</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.15">
@@ -3289,10 +3243,10 @@
         <v>63</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.15">
@@ -3300,10 +3254,10 @@
         <v>64</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.15">
@@ -3311,10 +3265,10 @@
         <v>65</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.15">
@@ -3328,10 +3282,10 @@
         <v>44</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.15">
@@ -3339,10 +3293,10 @@
         <v>67</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.15">
@@ -3350,10 +3304,10 @@
         <v>68</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.15">
@@ -3367,21 +3321,21 @@
         <v>154</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B108" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
@@ -3399,10 +3353,10 @@
         <v>177</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
@@ -3420,10 +3374,10 @@
         <v>199</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
@@ -3432,13 +3386,13 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B111" s="1" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
@@ -3447,24 +3401,24 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B112" s="1" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B113" s="1" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
@@ -3478,10 +3432,10 @@
         <v>147</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
@@ -3495,10 +3449,10 @@
         <v>139</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
@@ -3512,10 +3466,10 @@
         <v>161</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
@@ -3529,10 +3483,10 @@
         <v>184</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
@@ -3546,10 +3500,10 @@
         <v>190</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
@@ -3563,10 +3517,10 @@
         <v>204</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
@@ -3580,10 +3534,10 @@
         <v>152</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
@@ -3597,10 +3551,10 @@
         <v>92</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
@@ -3614,10 +3568,10 @@
         <v>227</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
@@ -3631,10 +3585,10 @@
         <v>123</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
@@ -3648,10 +3602,10 @@
         <v>169</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
@@ -3665,10 +3619,10 @@
         <v>115</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
@@ -3682,10 +3636,10 @@
         <v>107</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
@@ -3699,10 +3653,10 @@
         <v>211</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.15">
@@ -3716,21 +3670,21 @@
         <v>243</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B129" s="1" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.15">
@@ -3738,10 +3692,10 @@
         <v>80</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.15">
@@ -3749,10 +3703,10 @@
         <v>81</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.15">
@@ -3760,10 +3714,10 @@
         <v>82</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.15">
@@ -3777,10 +3731,10 @@
         <v>202</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.15">
@@ -3794,10 +3748,10 @@
         <v>128</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>254</v>
+        <v>397</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>294</v>
+        <v>397</v>
       </c>
       <c r="F141" s="1"/>
     </row>
@@ -3812,10 +3766,10 @@
         <v>112</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="F142" s="1"/>
     </row>
@@ -3830,10 +3784,10 @@
         <v>90</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>253</v>
+        <v>383</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
       <c r="F143" s="1"/>
     </row>
@@ -3848,10 +3802,10 @@
         <v>121</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="F144" s="1"/>
     </row>
@@ -3866,10 +3820,10 @@
         <v>137</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>256</v>
+        <v>385</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="F145" s="1"/>
     </row>
@@ -3884,10 +3838,10 @@
         <v>100</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>251</v>
+        <v>386</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="F146" s="1"/>
     </row>
@@ -3902,10 +3856,10 @@
         <v>131</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="F147" s="1"/>
     </row>
@@ -3920,10 +3874,10 @@
         <v>47</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>261</v>
+        <v>387</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="F148" s="1"/>
     </row>
@@ -3938,10 +3892,10 @@
         <v>69</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>264</v>
+        <v>388</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="F149" s="1"/>
     </row>
@@ -3956,10 +3910,10 @@
         <v>24</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>258</v>
+        <v>389</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="F150" s="1"/>
     </row>
@@ -3974,10 +3928,10 @@
         <v>16</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>257</v>
+        <v>390</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="F151" s="1"/>
     </row>
@@ -3992,10 +3946,10 @@
         <v>39</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>260</v>
+        <v>391</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="F152" s="1"/>
     </row>
@@ -4010,10 +3964,10 @@
         <v>77</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>265</v>
+        <v>392</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="F153" s="1"/>
     </row>
@@ -4028,10 +3982,10 @@
         <v>84</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>266</v>
+        <v>393</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="F154" s="1"/>
     </row>
@@ -4046,10 +4000,10 @@
         <v>62</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>263</v>
+        <v>394</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="F155" s="1"/>
     </row>
@@ -4064,10 +4018,10 @@
         <v>54</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>262</v>
+        <v>395</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="F156" s="1"/>
     </row>
@@ -4082,10 +4036,10 @@
         <v>31</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>259</v>
+        <v>396</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>413</v>
+        <v>396</v>
       </c>
       <c r="F157" s="1"/>
     </row>

</xml_diff>